<commit_message>
Cleaned all the categorical variables section code and adjusted the categories based on all input received; harmonized the continuous one; will try to do the merge
</commit_message>
<xml_diff>
--- a/continuous_L2_summary.xlsx
+++ b/continuous_L2_summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
   <si>
     <t xml:space="preserve">cont_indicatorcategory_l1</t>
   </si>
@@ -278,13 +278,10 @@
     <t xml:space="preserve">Clinical signs</t>
   </si>
   <si>
-    <t xml:space="preserve">39.0 to 39.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.0 to 37.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinical signs, unspecified when</t>
+    <t xml:space="preserve">37.0 to 39.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.0 to 37.8</t>
   </si>
   <si>
     <t xml:space="preserve">Blood pressure diastolic, value</t>
@@ -300,9 +297,6 @@
   </si>
   <si>
     <t xml:space="preserve">76.0 to 76.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.8 to 37.8</t>
   </si>
   <si>
     <t xml:space="preserve">Comorbidities</t>
@@ -2428,8 +2422,8 @@
       <c r="B37" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="21" t="n">
-        <v>1</v>
+      <c r="C37" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>61</v>
@@ -2446,16 +2440,16 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
         <v>90</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
         <v>91</v>
-      </c>
-      <c r="C38" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>92</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>39.35</v>
@@ -2475,132 +2469,132 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" t="s">
         <v>94</v>
-      </c>
-      <c r="I39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="21" t="n">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="C40" s="12" t="n">
+        <v>13</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
+      <c r="E40" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="G40" s="65" t="n">
+        <v>1.1</v>
+      </c>
       <c r="H40" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="I40" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="12" t="n">
-        <v>13</v>
+        <v>99</v>
+      </c>
+      <c r="C41" s="21" t="n">
+        <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>27</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>3.65</v>
+        <v>3</v>
       </c>
       <c r="F41" s="3" t="n">
-        <v>2.55</v>
+        <v>2</v>
       </c>
       <c r="G41" s="65" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="I41" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B42" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="21" t="n">
-        <v>1</v>
+      <c r="C42" s="6" t="n">
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E42" s="3" t="n">
-        <v>3</v>
+        <v>61.72</v>
       </c>
       <c r="F42" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G42" s="65" t="n">
-        <v>1</v>
+        <v>58.54</v>
+      </c>
+      <c r="G42" s="57" t="n">
+        <v>3.18</v>
       </c>
       <c r="H42" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="I42" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="6" t="n">
-        <v>35</v>
+        <v>104</v>
+      </c>
+      <c r="C43" s="21" t="n">
+        <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="3" t="n">
-        <v>61.72</v>
-      </c>
-      <c r="F43" s="3" t="n">
-        <v>58.54</v>
-      </c>
-      <c r="G43" s="57" t="n">
-        <v>3.18</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
       <c r="H43" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I43" t="s">
         <v>105</v>
@@ -2608,245 +2602,251 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" s="21" t="n">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="C44" s="13" t="n">
+        <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>11103</v>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>9591.33</v>
+      </c>
+      <c r="G44" s="32" t="n">
+        <v>1511.67</v>
+      </c>
       <c r="H44" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I44" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" s="13" t="n">
-        <v>11</v>
+        <v>110</v>
+      </c>
+      <c r="C45" s="17" t="n">
+        <v>5</v>
       </c>
       <c r="D45" t="s">
         <v>38</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>11103</v>
+        <v>828.5</v>
       </c>
       <c r="F45" s="3" t="n">
-        <v>9591.33</v>
-      </c>
-      <c r="G45" s="32" t="n">
-        <v>1511.67</v>
+        <v>361.9</v>
+      </c>
+      <c r="G45" s="37" t="n">
+        <v>466.6</v>
       </c>
       <c r="H45" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I45" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" s="17" t="n">
-        <v>5</v>
+        <v>113</v>
+      </c>
+      <c r="C46" s="19" t="n">
+        <v>3</v>
       </c>
       <c r="D46" t="s">
         <v>38</v>
       </c>
       <c r="E46" s="3" t="n">
-        <v>828.5</v>
+        <v>2860</v>
       </c>
       <c r="F46" s="3" t="n">
-        <v>361.9</v>
-      </c>
-      <c r="G46" s="37" t="n">
-        <v>466.6</v>
+        <v>1573</v>
+      </c>
+      <c r="G46" s="33" t="n">
+        <v>1287</v>
       </c>
       <c r="H46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" s="19" t="n">
-        <v>3</v>
+        <v>116</v>
+      </c>
+      <c r="C47" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>2860</v>
+        <v>1956</v>
       </c>
       <c r="F47" s="3" t="n">
-        <v>1573</v>
-      </c>
-      <c r="G47" s="33" t="n">
-        <v>1287</v>
+        <v>1450</v>
+      </c>
+      <c r="G47" s="36" t="n">
+        <v>506</v>
       </c>
       <c r="H47" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I47" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C48" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E48" s="3" t="n">
-        <v>1956</v>
+        <v>59266</v>
       </c>
       <c r="F48" s="3" t="n">
-        <v>1450</v>
-      </c>
-      <c r="G48" s="36" t="n">
-        <v>506</v>
+        <v>36452</v>
+      </c>
+      <c r="G48" s="28" t="n">
+        <v>22814</v>
       </c>
       <c r="H48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C49" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>59266</v>
+        <v>10429</v>
       </c>
       <c r="F49" s="3" t="n">
-        <v>36452</v>
-      </c>
-      <c r="G49" s="28" t="n">
-        <v>22814</v>
+        <v>8308</v>
+      </c>
+      <c r="G49" s="31" t="n">
+        <v>2121</v>
       </c>
       <c r="H49" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I49" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50" s="20" t="n">
-        <v>2</v>
+        <v>126</v>
+      </c>
+      <c r="C50" s="21" t="n">
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
-      </c>
-      <c r="E50" s="3" t="n">
-        <v>10429</v>
-      </c>
-      <c r="F50" s="3" t="n">
-        <v>8308</v>
-      </c>
-      <c r="G50" s="31" t="n">
-        <v>2121</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
       <c r="H50" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I50" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C51" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>119</v>
-      </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>1112</v>
+      </c>
+      <c r="F51" s="3" t="n">
+        <v>654</v>
+      </c>
+      <c r="G51" s="37" t="n">
+        <v>458</v>
+      </c>
       <c r="H51" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="I51" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C52" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>1112</v>
+        <v>722</v>
       </c>
       <c r="F52" s="3" t="n">
-        <v>654</v>
-      </c>
-      <c r="G52" s="37" t="n">
-        <v>458</v>
+        <v>404</v>
+      </c>
+      <c r="G52" s="39" t="n">
+        <v>318</v>
       </c>
       <c r="H52" t="s">
         <v>27</v>
@@ -2857,25 +2857,25 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>722</v>
+        <v>1066</v>
       </c>
       <c r="F53" s="3" t="n">
-        <v>404</v>
-      </c>
-      <c r="G53" s="39" t="n">
-        <v>318</v>
+        <v>652</v>
+      </c>
+      <c r="G53" s="38" t="n">
+        <v>414</v>
       </c>
       <c r="H53" t="s">
         <v>27</v>
@@ -2886,25 +2886,25 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C54" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>1066</v>
+        <v>257</v>
       </c>
       <c r="F54" s="3" t="n">
-        <v>652</v>
-      </c>
-      <c r="G54" s="38" t="n">
-        <v>414</v>
+        <v>183</v>
+      </c>
+      <c r="G54" s="43" t="n">
+        <v>74</v>
       </c>
       <c r="H54" t="s">
         <v>27</v>
@@ -2915,152 +2915,152 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" t="s">
         <v>134</v>
       </c>
-      <c r="C55" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>119</v>
-      </c>
-      <c r="E55" s="3" t="n">
-        <v>257</v>
-      </c>
-      <c r="F55" s="3" t="n">
-        <v>183</v>
-      </c>
-      <c r="G55" s="43" t="n">
-        <v>74</v>
-      </c>
-      <c r="H55" t="s">
-        <v>27</v>
-      </c>
       <c r="I55" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C56" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I56" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C57" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>119</v>
-      </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="66" t="n">
+        <v>0</v>
+      </c>
       <c r="H57" t="s">
-        <v>139</v>
+        <v>27</v>
       </c>
       <c r="I57" t="s">
-        <v>140</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
-        <v>119</v>
-      </c>
-      <c r="E58" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" s="66" t="n">
-        <v>0</v>
-      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
       <c r="H58" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="I58" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C59" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
-      </c>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>68.1</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>203.1</v>
+      </c>
+      <c r="G59" s="25" t="n">
+        <v>-135</v>
+      </c>
       <c r="H59" t="s">
-        <v>144</v>
+        <v>27</v>
       </c>
       <c r="I59" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C60" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>68.1</v>
+        <v>0</v>
       </c>
       <c r="F60" s="3" t="n">
-        <v>203.1</v>
-      </c>
-      <c r="G60" s="25" t="n">
-        <v>-135</v>
+        <v>0</v>
+      </c>
+      <c r="G60" s="66" t="n">
+        <v>0</v>
       </c>
       <c r="H60" t="s">
         <v>27</v>
@@ -3071,25 +3071,25 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C61" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E61" s="3" t="n">
-        <v>0</v>
+        <v>1189</v>
       </c>
       <c r="F61" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="66" t="n">
-        <v>0</v>
+        <v>309</v>
+      </c>
+      <c r="G61" s="34" t="n">
+        <v>880</v>
       </c>
       <c r="H61" t="s">
         <v>27</v>
@@ -3100,175 +3100,175 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="B62" t="s">
         <v>148</v>
       </c>
-      <c r="C62" s="21" t="n">
-        <v>1</v>
+      <c r="C62" s="4" t="n">
+        <v>45</v>
       </c>
       <c r="D62" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="E62" s="3" t="n">
-        <v>1189</v>
+        <v>30.65</v>
       </c>
       <c r="F62" s="3" t="n">
-        <v>309</v>
-      </c>
-      <c r="G62" s="34" t="n">
-        <v>880</v>
+        <v>17.11</v>
+      </c>
+      <c r="G62" s="50" t="n">
+        <v>13.53</v>
       </c>
       <c r="H62" t="s">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="I62" t="s">
-        <v>27</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
-      </c>
-      <c r="C63" s="4" t="n">
-        <v>45</v>
+        <v>151</v>
+      </c>
+      <c r="C63" s="16" t="n">
+        <v>6</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>30.65</v>
+        <v>14.37</v>
       </c>
       <c r="F63" s="3" t="n">
-        <v>17.11</v>
-      </c>
-      <c r="G63" s="50" t="n">
-        <v>13.53</v>
+        <v>5.89</v>
+      </c>
+      <c r="G63" s="52" t="n">
+        <v>8.48</v>
       </c>
       <c r="H63" t="s">
-        <v>151</v>
+        <v>27</v>
       </c>
       <c r="I63" t="s">
-        <v>152</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B64" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I64" t="s">
         <v>153</v>
-      </c>
-      <c r="C64" s="16" t="n">
-        <v>6</v>
-      </c>
-      <c r="D64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="3" t="n">
-        <v>14.37</v>
-      </c>
-      <c r="F64" s="3" t="n">
-        <v>5.89</v>
-      </c>
-      <c r="G64" s="52" t="n">
-        <v>8.48</v>
-      </c>
-      <c r="H64" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B65" t="s">
-        <v>154</v>
-      </c>
-      <c r="C65" s="21" t="n">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="C65" s="5" t="n">
+        <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>27</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="E65" s="3" t="n">
+        <v>33.18</v>
+      </c>
+      <c r="F65" s="3" t="n">
+        <v>20.01</v>
+      </c>
+      <c r="G65" s="50" t="n">
+        <v>13.17</v>
+      </c>
       <c r="H65" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="I65" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B66" t="s">
-        <v>157</v>
-      </c>
-      <c r="C66" s="5" t="n">
-        <v>37</v>
+        <v>158</v>
+      </c>
+      <c r="C66" s="16" t="n">
+        <v>6</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>33.18</v>
+        <v>11.9</v>
       </c>
       <c r="F66" s="3" t="n">
-        <v>20.01</v>
-      </c>
-      <c r="G66" s="50" t="n">
-        <v>13.17</v>
+        <v>7.65</v>
+      </c>
+      <c r="G66" s="56" t="n">
+        <v>4.25</v>
       </c>
       <c r="H66" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I66" t="s">
-        <v>159</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
-        <v>160</v>
-      </c>
-      <c r="C67" s="16" t="n">
-        <v>6</v>
+        <v>161</v>
+      </c>
+      <c r="C67" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="D67" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>11.9</v>
+        <v>3.3</v>
       </c>
       <c r="F67" s="3" t="n">
-        <v>7.65</v>
-      </c>
-      <c r="G67" s="56" t="n">
-        <v>4.25</v>
+        <v>1.1</v>
+      </c>
+      <c r="G67" s="60" t="n">
+        <v>2.2</v>
       </c>
       <c r="H67" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I67" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B68" t="s">
         <v>163</v>
@@ -3280,53 +3280,53 @@
         <v>11</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="F68" s="3" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="G68" s="60" t="n">
-        <v>2.2</v>
+        <v>9.4</v>
+      </c>
+      <c r="G68" s="29" t="n">
+        <v>-4.4</v>
       </c>
       <c r="H68" t="s">
         <v>164</v>
       </c>
       <c r="I68" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B69" t="s">
-        <v>165</v>
-      </c>
-      <c r="C69" s="20" t="n">
-        <v>2</v>
+        <v>166</v>
+      </c>
+      <c r="C69" s="21" t="n">
+        <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>167</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="F69" s="3" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="G69" s="29" t="n">
-        <v>-4.4</v>
+        <v>0</v>
+      </c>
+      <c r="G69" s="42" t="n">
+        <v>123</v>
       </c>
       <c r="H69" t="s">
-        <v>166</v>
+        <v>27</v>
       </c>
       <c r="I69" t="s">
-        <v>167</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B70" t="s">
         <v>168</v>
@@ -3335,16 +3335,16 @@
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>169</v>
+        <v>27</v>
       </c>
       <c r="E70" s="3" t="n">
-        <v>123</v>
+        <v>2.4</v>
       </c>
       <c r="F70" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" s="42" t="n">
-        <v>123</v>
+        <v>1</v>
+      </c>
+      <c r="G70" s="63" t="n">
+        <v>1.4</v>
       </c>
       <c r="H70" t="s">
         <v>27</v>
@@ -3355,25 +3355,25 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C71" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>27</v>
+        <v>167</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>2.4</v>
+        <v>28.1</v>
       </c>
       <c r="F71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G71" s="63" t="n">
-        <v>1.4</v>
+        <v>13.4</v>
+      </c>
+      <c r="G71" s="49" t="n">
+        <v>14.7</v>
       </c>
       <c r="H71" t="s">
         <v>27</v>
@@ -3384,39 +3384,33 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C72" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>169</v>
-      </c>
-      <c r="E72" s="3" t="n">
-        <v>28.1</v>
-      </c>
-      <c r="F72" s="3" t="n">
-        <v>13.4</v>
-      </c>
-      <c r="G72" s="49" t="n">
-        <v>14.7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
       <c r="H72" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="I72" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B73" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C73" s="21" t="n">
         <v>1</v>
@@ -3424,22 +3418,28 @@
       <c r="D73" t="s">
         <v>11</v>
       </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
+      <c r="E73" s="3" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="F73" s="3" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G73" s="56" t="n">
+        <v>4</v>
+      </c>
       <c r="H73" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="I73" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C74" s="21" t="n">
         <v>1</v>
@@ -3447,25 +3447,19 @@
       <c r="D74" t="s">
         <v>11</v>
       </c>
-      <c r="E74" s="3" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="F74" s="3" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="G74" s="56" t="n">
-        <v>4</v>
-      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
       <c r="H74" t="s">
-        <v>27</v>
+        <v>173</v>
       </c>
       <c r="I74" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B75" t="s">
         <v>174</v>
@@ -3480,18 +3474,18 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="I75" t="s">
-        <v>167</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C76" s="21" t="n">
         <v>1</v>
@@ -3503,15 +3497,15 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" t="s">
-        <v>21</v>
+        <v>176</v>
       </c>
       <c r="I76" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B77" t="s">
         <v>177</v>
@@ -3522,207 +3516,213 @@
       <c r="D77" t="s">
         <v>11</v>
       </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
+      <c r="E77" s="3" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="F77" s="3" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="G77" s="30" t="n">
+        <v>-4.1</v>
+      </c>
       <c r="H77" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="I77" t="s">
-        <v>175</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C78" s="21" t="n">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="3" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="F78" s="3" t="n">
-        <v>9.3</v>
-      </c>
-      <c r="G78" s="30" t="n">
-        <v>-4.1</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
       <c r="H78" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="I78" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="B79" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="21" t="n">
-        <v>1</v>
+      <c r="C79" s="11" t="n">
+        <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>169</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>265.45</v>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>36.64</v>
+      </c>
+      <c r="G79" s="40" t="n">
+        <v>228.81</v>
+      </c>
       <c r="H79" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="I79" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B80" t="s">
-        <v>182</v>
-      </c>
-      <c r="C80" s="11" t="n">
-        <v>14</v>
+        <v>183</v>
+      </c>
+      <c r="C80" s="21" t="n">
+        <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>38</v>
-      </c>
-      <c r="E80" s="3" t="n">
-        <v>265.45</v>
-      </c>
-      <c r="F80" s="3" t="n">
-        <v>36.64</v>
-      </c>
-      <c r="G80" s="40" t="n">
-        <v>228.81</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
       <c r="H80" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="I80" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B81" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
         <v>185</v>
-      </c>
-      <c r="C81" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D81" t="s">
-        <v>169</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
       <c r="I81" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B82" t="s">
-        <v>186</v>
-      </c>
-      <c r="C82" s="21" t="n">
-        <v>1</v>
+        <v>187</v>
+      </c>
+      <c r="C82" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>187</v>
-      </c>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
+        <v>188</v>
+      </c>
+      <c r="E82" s="3" t="n">
+        <v>1852.08</v>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>2841.78</v>
+      </c>
+      <c r="G82" s="22" t="n">
+        <v>-989.7</v>
+      </c>
       <c r="H82" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
       <c r="I82" t="s">
-        <v>27</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B83" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C83" s="20" t="n">
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>1852.08</v>
+        <v>33.59</v>
       </c>
       <c r="F83" s="3" t="n">
-        <v>2841.78</v>
-      </c>
-      <c r="G83" s="22" t="n">
-        <v>-989.7</v>
+        <v>36.27</v>
+      </c>
+      <c r="G83" s="35" t="n">
+        <v>-2.68</v>
       </c>
       <c r="H83" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I83" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B84" t="s">
-        <v>193</v>
-      </c>
-      <c r="C84" s="20" t="n">
-        <v>2</v>
+        <v>195</v>
+      </c>
+      <c r="C84" s="21" t="n">
+        <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>194</v>
+        <v>27</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>33.59</v>
+        <v>5.6</v>
       </c>
       <c r="F84" s="3" t="n">
-        <v>36.27</v>
-      </c>
-      <c r="G84" s="35" t="n">
-        <v>-2.68</v>
+        <v>6.98</v>
+      </c>
+      <c r="G84" s="44" t="n">
+        <v>-1.38</v>
       </c>
       <c r="H84" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
       <c r="I84" t="s">
-        <v>196</v>
+        <v>27</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B85" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C85" s="21" t="n">
         <v>1</v>
@@ -3731,13 +3731,13 @@
         <v>27</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>5.6</v>
+        <v>6.63</v>
       </c>
       <c r="F85" s="3" t="n">
-        <v>6.98</v>
-      </c>
-      <c r="G85" s="44" t="n">
-        <v>-1.38</v>
+        <v>7.78</v>
+      </c>
+      <c r="G85" s="45" t="n">
+        <v>-1.15</v>
       </c>
       <c r="H85" t="s">
         <v>27</v>
@@ -3748,10 +3748,10 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B86" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C86" s="21" t="n">
         <v>1</v>
@@ -3760,13 +3760,13 @@
         <v>27</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>6.63</v>
+        <v>18</v>
       </c>
       <c r="F86" s="3" t="n">
-        <v>7.78</v>
-      </c>
-      <c r="G86" s="45" t="n">
-        <v>-1.15</v>
+        <v>16.5</v>
+      </c>
+      <c r="G86" s="63" t="n">
+        <v>1.5</v>
       </c>
       <c r="H86" t="s">
         <v>27</v>
@@ -3777,146 +3777,146 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B87" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" t="s">
         <v>199</v>
       </c>
-      <c r="C87" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D87" t="s">
-        <v>27</v>
-      </c>
-      <c r="E87" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="F87" s="3" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="G87" s="63" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="H87" t="s">
-        <v>27</v>
-      </c>
       <c r="I87" t="s">
-        <v>27</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="B88" t="s">
-        <v>200</v>
-      </c>
-      <c r="C88" s="21" t="n">
-        <v>1</v>
+        <v>202</v>
+      </c>
+      <c r="C88" s="7" t="n">
+        <v>28</v>
       </c>
       <c r="D88" t="s">
-        <v>27</v>
-      </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="E88" s="3" t="n">
+        <v>23.92</v>
+      </c>
+      <c r="F88" s="3" t="n">
+        <v>14.92</v>
+      </c>
+      <c r="G88" s="51" t="n">
+        <v>9</v>
+      </c>
       <c r="H88" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I88" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B89" t="s">
-        <v>204</v>
-      </c>
-      <c r="C89" s="7" t="n">
-        <v>28</v>
+        <v>205</v>
+      </c>
+      <c r="C89" s="14" t="n">
+        <v>8</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>23.92</v>
+        <v>7.7</v>
       </c>
       <c r="F89" s="3" t="n">
-        <v>14.92</v>
-      </c>
-      <c r="G89" s="51" t="n">
-        <v>9</v>
+        <v>5.22</v>
+      </c>
+      <c r="G89" s="59" t="n">
+        <v>2.48</v>
       </c>
       <c r="H89" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I89" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B90" t="s">
-        <v>207</v>
-      </c>
-      <c r="C90" s="14" t="n">
-        <v>8</v>
+        <v>208</v>
+      </c>
+      <c r="C90" s="18" t="n">
+        <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>7.7</v>
+        <v>101.14</v>
       </c>
       <c r="F90" s="3" t="n">
-        <v>5.22</v>
-      </c>
-      <c r="G90" s="59" t="n">
-        <v>2.48</v>
+        <v>169.09</v>
+      </c>
+      <c r="G90" s="26" t="n">
+        <v>-67.95</v>
       </c>
       <c r="H90" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I90" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B91" t="s">
-        <v>210</v>
-      </c>
-      <c r="C91" s="18" t="n">
-        <v>4</v>
+        <v>211</v>
+      </c>
+      <c r="C91" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E91" s="3" t="n">
-        <v>101.14</v>
+        <v>102.4</v>
       </c>
       <c r="F91" s="3" t="n">
-        <v>169.09</v>
-      </c>
-      <c r="G91" s="26" t="n">
-        <v>-67.95</v>
+        <v>251.6</v>
+      </c>
+      <c r="G91" s="24" t="n">
+        <v>-149.2</v>
       </c>
       <c r="H91" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I91" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B92" t="s">
         <v>213</v>
@@ -3928,53 +3928,47 @@
         <v>11</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>102.4</v>
+        <v>14.95</v>
       </c>
       <c r="F92" s="3" t="n">
-        <v>251.6</v>
-      </c>
-      <c r="G92" s="24" t="n">
-        <v>-149.2</v>
+        <v>8.6</v>
+      </c>
+      <c r="G92" s="53" t="n">
+        <v>6.35</v>
       </c>
       <c r="H92" t="s">
-        <v>214</v>
+        <v>27</v>
       </c>
       <c r="I92" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B93" t="s">
-        <v>215</v>
-      </c>
-      <c r="C93" s="20" t="n">
-        <v>2</v>
+        <v>214</v>
+      </c>
+      <c r="C93" s="21" t="n">
+        <v>1</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
       </c>
-      <c r="E93" s="3" t="n">
-        <v>14.95</v>
-      </c>
-      <c r="F93" s="3" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="G93" s="53" t="n">
-        <v>6.35</v>
-      </c>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
       <c r="H93" t="s">
-        <v>27</v>
+        <v>215</v>
       </c>
       <c r="I93" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B94" t="s">
         <v>216</v>
@@ -3992,15 +3986,15 @@
         <v>217</v>
       </c>
       <c r="I94" t="s">
-        <v>59</v>
+        <v>218</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B95" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C95" s="21" t="n">
         <v>1</v>
@@ -4012,52 +4006,28 @@
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I95" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B96" t="s">
         <v>221</v>
       </c>
-      <c r="C96" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D96" t="s">
-        <v>11</v>
-      </c>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" t="s">
-        <v>222</v>
-      </c>
-      <c r="I96" t="s">
-        <v>223</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A36"/>
-    <mergeCell ref="A37:A37"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A68:A79"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="A83:A88"/>
-    <mergeCell ref="A89:A96"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A78"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="A88:A95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>